<commit_message>
Adding data points for new participant
</commit_message>
<xml_diff>
--- a/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
+++ b/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\NY Trip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\Dev\GitHub\antitheos.github.io\HistoryMovesBrooklyn\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Carmen" sheetId="1" r:id="rId1"/>
-    <sheet name="Barbara" sheetId="2" r:id="rId2"/>
+    <sheet name="Barbara" sheetId="2" r:id="rId1"/>
+    <sheet name="Carmen" sheetId="1" r:id="rId2"/>
+    <sheet name="Carol" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="172">
   <si>
     <t>Location</t>
   </si>
@@ -428,6 +429,129 @@
   </si>
   <si>
     <t>1368 Fulton St, Brooklyn, NY 11216</t>
+  </si>
+  <si>
+    <t>Brooklyn New York ­ Pitkin between Powell and Junius ­ born and grew up</t>
+  </si>
+  <si>
+    <t>PS233 in Brownsville on Christopher ­ school</t>
+  </si>
+  <si>
+    <t>Queens­­ Jamaica, Queens ­ school 292</t>
+  </si>
+  <si>
+    <t>PS292 on Wyona between Pitkin and Belmont [Vermont] ­ school</t>
+  </si>
+  <si>
+    <t>Maxwell Vocational High School</t>
+  </si>
+  <si>
+    <t>GED school on Nostrand and Macon</t>
+  </si>
+  <si>
+    <t>born 61</t>
+  </si>
+  <si>
+    <t>diagnosed at 48 ­ 2010 ­ Brookdale Hospital</t>
+  </si>
+  <si>
+    <t>57 Willoughby Housing Works</t>
+  </si>
+  <si>
+    <t>Housing Works on Pitkin between Fountain and Crystal in East New York</t>
+  </si>
+  <si>
+    <t>Star Clinic</t>
+  </si>
+  <si>
+    <t>pharmacy</t>
+  </si>
+  <si>
+    <t>daughters house</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>I worked at Home Health Aide for 13 years,</t>
+  </si>
+  <si>
+    <t>church at home</t>
+  </si>
+  <si>
+    <t>67 Willoughby Street ­ sent after diagnosis for support ­ 2010 ­ Downtown Brooklyn. ­</t>
+  </si>
+  <si>
+    <t>best place can be</t>
+  </si>
+  <si>
+    <t>Parkside ­ store ­ met gloria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>Born, grew up</t>
+  </si>
+  <si>
+    <t>Daughter</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>9301 Avenue B, Brooklyn, NY 11236</t>
+  </si>
+  <si>
+    <t>301 Vermont St, Brooklyn, NY 11207</t>
+  </si>
+  <si>
+    <t>Junior High School 292 Margaret S Douglas</t>
+  </si>
+  <si>
+    <t>P.S. 233 Langston Hughes</t>
+  </si>
+  <si>
+    <t>145 Pennsylvan Ave, Brooklyn, NY 11207</t>
+  </si>
+  <si>
+    <t>W. H. Maxwell Career And Technical Education High School</t>
+  </si>
+  <si>
+    <t>Brookdale Hospital and Medical Center</t>
+  </si>
+  <si>
+    <t>57 Willoughby St
+Brooklyn, NY 11201</t>
+  </si>
+  <si>
+    <t>67 Willoughby St
+Brooklyn, NY 11201</t>
+  </si>
+  <si>
+    <t>Brooklyn Adult Learning Center</t>
+  </si>
+  <si>
+    <t>475 Nostrand Ave, Brooklyn, NY 11216</t>
+  </si>
+  <si>
+    <t>Health Center</t>
+  </si>
+  <si>
+    <t>2640 Pitkin Ave
+Brooklyn, NY 11208</t>
+  </si>
+  <si>
+    <t>Housing Works, East New York Community Health Center</t>
+  </si>
+  <si>
+    <t>Housing Works</t>
   </si>
 </sst>
 </file>
@@ -787,436 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.53125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.1328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.46484375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="9.06640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="40" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="1">
-        <v>40.655434999999997</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-73.947912000000002</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1">
-        <v>40.679687199999996</v>
-      </c>
-      <c r="F3" s="1">
-        <v>-73.980439399999995</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="40" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="1">
-        <v>40.781952500000003</v>
-      </c>
-      <c r="F4" s="1">
-        <v>-74.061342800000006</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1971</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1992</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1974</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1975</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1982</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="1">
-        <v>40.679687199999996</v>
-      </c>
-      <c r="F11" s="1">
-        <v>-73.980439399999995</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="40" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1">
-        <v>40.667614700000001</v>
-      </c>
-      <c r="F12" s="1">
-        <v>-73.980696199999997</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="40" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="1">
-        <v>40.655434999999997</v>
-      </c>
-      <c r="F13" s="1">
-        <v>-73.947912000000002</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1988</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="40" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1">
-        <v>40.764690000000002</v>
-      </c>
-      <c r="F15" s="1">
-        <v>-73.940189000000004</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="1">
-        <v>40.752473000000002</v>
-      </c>
-      <c r="F18" s="1">
-        <v>-73.993654699999993</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1909,4 +1607,830 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40.655434999999997</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-73.947912000000002</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40.679687199999996</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-73.980439399999995</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40.781952500000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-74.061342800000006</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1971</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1992</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1974</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1975</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1982</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="1">
+        <v>40.679687199999996</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-73.980439399999995</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1">
+        <v>40.667614700000001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-73.980696199999997</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>40.655434999999997</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-73.947912000000002</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1988</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1">
+        <v>40.764690000000002</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-73.940189000000004</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1">
+        <v>40.752473000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-73.993654699999993</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40.655434999999997</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-73.947912000000002</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40.651400700000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-73.9139658</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40.671613200000003</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-73.893389900000003</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40.671613200000003</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-73.893389900000003</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="B7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40.673848800000002</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-73.8961726</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1">
+        <v>40.681445199999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-73.949605700000006</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="1">
+        <v>40.655094200000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-73.912631300000001</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="1">
+        <v>40.6924992</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-73.986506300000002</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="B13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1">
+        <v>40.752473000000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-73.993654699999993</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="40" x14ac:dyDescent="0.45">
+      <c r="B19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="1">
+        <v>40.692163999999998</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-73.987764600000006</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B20" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B23" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix miscoded lat & long
</commit_message>
<xml_diff>
--- a/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
+++ b/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="173">
   <si>
     <t>Location</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>Housing Works</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pitkin between Powell and Junius, Brooklyn, NY 11212</t>
   </si>
 </sst>
 </file>
@@ -913,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1614,7 +1617,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:I18"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1682,10 +1685,10 @@
         <v>49</v>
       </c>
       <c r="E2" s="1">
-        <v>40.655434999999997</v>
+        <v>40.6554</v>
       </c>
       <c r="F2" s="1">
-        <v>-73.947912000000002</v>
+        <v>-73.945700000000002</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
@@ -1905,10 +1908,10 @@
         <v>49</v>
       </c>
       <c r="E13" s="1">
-        <v>40.655434999999997</v>
+        <v>40.6554</v>
       </c>
       <c r="F13" s="1">
-        <v>-73.947912000000002</v>
+        <v>-73.945700000000002</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>26</v>
@@ -2039,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2105,10 +2108,10 @@
         <v>49</v>
       </c>
       <c r="E2" s="1">
-        <v>40.655434999999997</v>
+        <v>40.6554</v>
       </c>
       <c r="F2" s="1">
-        <v>-73.947912000000002</v>
+        <v>-73.945700000000002</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
@@ -2117,9 +2120,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>132</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40.670837800000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-73.903683299999997</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
@@ -2315,6 +2327,12 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>169</v>
+      </c>
+      <c r="E12" s="1">
+        <v>40.674765999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-73.874803499999999</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Adding images for use in wiki
</commit_message>
<xml_diff>
--- a/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
+++ b/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Barbara" sheetId="2" r:id="rId1"/>
     <sheet name="Carmen" sheetId="1" r:id="rId2"/>
     <sheet name="Carol" sheetId="3" r:id="rId3"/>
+    <sheet name="Cheri" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="213">
   <si>
     <t>Location</t>
   </si>
@@ -555,6 +556,126 @@
   </si>
   <si>
     <t xml:space="preserve"> Pitkin between Powell and Junius, Brooklyn, NY 11212</t>
+  </si>
+  <si>
+    <t>Union Hospital in Brooklyn</t>
+  </si>
+  <si>
+    <t>birthday ­ 12, 1971.</t>
+  </si>
+  <si>
+    <t>William H. Maxwell High School</t>
+  </si>
+  <si>
+    <t>New York City Transit depot ­ mom worked as bus driver B20</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson High School</t>
+  </si>
+  <si>
+    <t>Kingdom Hall ­ Jehovah’s Witness</t>
+  </si>
+  <si>
+    <t>1988 ­ GED</t>
+  </si>
+  <si>
+    <t>medical malpractice law firm ­ where/job?</t>
+  </si>
+  <si>
+    <t>living where with husband ­ 94</t>
+  </si>
+  <si>
+    <t>pregnant test/diagnosis ­ where? ­ 94</t>
+  </si>
+  <si>
+    <t>Woods Program in 1994 ­ care program where</t>
+  </si>
+  <si>
+    <t>clinic ­ where ­ ?</t>
+  </si>
+  <si>
+    <t>Crown Heights ­ where dad lived</t>
+  </si>
+  <si>
+    <t>Rikers ­ prison ­ husband</t>
+  </si>
+  <si>
+    <t>living with grandmother ­ first child born ­ where</t>
+  </si>
+  <si>
+    <t>Brookdale Hospital ­ 98 ­ high blood pressure</t>
+  </si>
+  <si>
+    <t>Husband Aunts house ­ not allowed to share utensils ­ 94</t>
+  </si>
+  <si>
+    <t>church, where ­</t>
+  </si>
+  <si>
+    <t>Cheri</t>
+  </si>
+  <si>
+    <t>Born</t>
+  </si>
+  <si>
+    <t>Worship</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>husband</t>
+  </si>
+  <si>
+    <t>Crown Heights</t>
+  </si>
+  <si>
+    <t>diagnosis</t>
+  </si>
+  <si>
+    <t>Linden Houses, East New York ­ grew up here ­ four buildings that’s on a square Four Corners</t>
+  </si>
+  <si>
+    <t>Union Hospital</t>
+  </si>
+  <si>
+    <t>Linden Houses</t>
+  </si>
+  <si>
+    <t>child, mother</t>
+  </si>
+  <si>
+    <t>Husband's Aunt</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Prison</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Union Community Health Center, 260 E 188th St, Bronx, NY 10458, United States</t>
+  </si>
+  <si>
+    <t>145 Pennsylvania Ave, Brooklyn, NY 11207, United States</t>
+  </si>
+  <si>
+    <t>400 Pennsylvania Ave, Brooklyn, NY 11207</t>
+  </si>
+  <si>
+    <t>5201 Foster Avenue, Brooklyn, NY 11203</t>
+  </si>
+  <si>
+    <t>Rikers Island, NY, United States</t>
+  </si>
+  <si>
+    <t>Rikers Island</t>
+  </si>
+  <si>
+    <t>914 Van Siclen Ave, Brooklyn, NY 11207</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1738,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="D7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2042,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2451,4 +2572,424 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="66.349999999999994" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40.860785800000002</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-73.895989299999997</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40.673837200000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-73.896076800000003</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40.666868689130801</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-73.895242411114495</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40.657683909089997</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-73.884378949702807</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="1">
+        <v>40.640131529287601</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-73.926970855819704</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1994</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="1">
+        <v>40.792120500295397</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-73.886439153442296</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="40" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="1">
+        <v>40.655066400000003</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-73.912579300000004</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="26.8" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1994</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for roads, maps and locations
Show roads
Show multiple quotes at single location
Add extra quotes
</commit_message>
<xml_diff>
--- a/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
+++ b/HistoryMovesBrooklyn/Data/indexedcontent.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18426" windowHeight="9266"/>
   </bookViews>
   <sheets>
     <sheet name="Barbara" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="212">
   <si>
     <t>Location</t>
   </si>
@@ -220,91 +220,19 @@
     <t>Barbara</t>
   </si>
   <si>
-    <t>1958 East New York</t>
-  </si>
-  <si>
     <t>Fulton Street, 1557, Albany and Kingston</t>
   </si>
   <si>
-    <t>Alabama Avenue and New Lots Avenue and Hegemony Avenue 60s</t>
-  </si>
-  <si>
     <t>Bedford Stuyvesant</t>
   </si>
   <si>
-    <t>’60 to ’64 to East New York-Hegeman Avenue between Alabama and Malta.</t>
-  </si>
-  <si>
-    <t>PS213</t>
-  </si>
-  <si>
-    <t>PS190</t>
-  </si>
-  <si>
-    <t>Brooklyn NY</t>
-  </si>
-  <si>
-    <t>70s - 1975 - Brookdale Hospital</t>
-  </si>
-  <si>
-    <t>84-85 - 59th Street and Columbus - Clinic</t>
-  </si>
-  <si>
-    <t>96th Street and Clarkson to Kings County Hospital - 86 - Clinic</t>
-  </si>
-  <si>
-    <t>Amityville, Long Island - visit daughter in foster care</t>
-  </si>
-  <si>
-    <t>King’s County - daughter physc. treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holliswood Hospital in Queens - daughter physc. treatment </t>
-  </si>
-  <si>
-    <t>Red Cross put me in hotel</t>
-  </si>
-  <si>
-    <t>ACS - Kings County, the F Building or K Building by Albany - entered program drug treatment</t>
-  </si>
-  <si>
     <t>Mobile Alabama 2003</t>
   </si>
   <si>
-    <t>Rochester and Dean Street  - met Magic Johnson</t>
-  </si>
-  <si>
-    <t>Gold Street, downtown - Joyce McDonald from the Church of the Open Door - AIDS Minstry</t>
-  </si>
-  <si>
-    <t>Brownsville, Brooklyn - live - now (18 years)</t>
-  </si>
-  <si>
     <t>Staten Island - daughters home</t>
   </si>
   <si>
     <t>NA or AA meeting</t>
-  </si>
-  <si>
-    <t>Still I Rise, at Restoration  - group meeting</t>
-  </si>
-  <si>
-    <t>89 - positive assessment</t>
-  </si>
-  <si>
-    <t>99 started medication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interfaith - Hospital (next to drug house) - </t>
-  </si>
-  <si>
-    <t>Interfaith - Hospital (next to drug house) - 2000</t>
-  </si>
-  <si>
-    <t>Downstate - hospital HPV - 89 to 88</t>
-  </si>
-  <si>
-    <t>Downstate - hospital - 99 - 2016</t>
   </si>
   <si>
     <t>70s - 1975</t>
@@ -676,6 +604,83 @@
   </si>
   <si>
     <t>914 Van Siclen Ave, Brooklyn, NY 11207</t>
+  </si>
+  <si>
+    <t>I grew up in East New York, matter of fact, I was born and raised right there on Fulton Street, 1557, between Albany and Kingston.  I was born in ’58 so I'm young.</t>
+  </si>
+  <si>
+    <t>I grew up in East New York, I grew up on Alabama [Avenue] between New Lots [Avenue] and Hegeman [Avenue] in the ‘60s.
+Um, back then, it was so much different than what it is today.  Back then growing up when they say it takes a village to raise a child, they meant it back then; they just use the phrases today.  Because back then when we used to have block parties, all the families get together and stuff like that, everybody had one long table and we ate off that table, all the kids played together.  I used to just beat up all the kids; I used to like that part a lot, I did.  They couldn't beat me at nothing.  Skelly, riding a bike, you understand they couldn't (laughter) beat me at nothing.  I'm a challenger, I still am.  I’m a challenger.</t>
+  </si>
+  <si>
+    <t>When I moved right around the corner I went to 190, which was a school, I think I graduated – no, when I had a graduation dress on, they put me out.  You know?  See back in them days they really thought that children were bad, the ADHD and all that kind of stuff because of our behavior.  My behavior back then…I didn't know how to say Mommy, Daddy.  My right eye I can't really see out of.  Um, I can't keep up with the classroom because it takes me longer to read this sentence than the other children.  So not wanting to be the dumb child, I became the clown.  So I disturbed the whole class with my jokes and my attitude.  And then some days I’d just sit in the bathroom until the principal come and get me out…or they call my parents and they come get me out.  But nobody asked me the question – can you comprehend?  Back then nobody asked me.  So I didn't like school, I didn't want to go to school because I was just sitting in…nobody knew to ask me – can you keep up?  Maybe this classroom’s not for you; maybe you need to be in a special ed class; nobody asked me so I didn't learn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I went to PS213.  See back then, I think they still do it, I’m not really sure, it all depended on what side of the street you lived on.  So since I was on a certain side of the street, I went to 213.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I went to, well when I first left Bedford Stuyvesant my mother and I moved in from ’60 to ’64 to East New York, we moved on Hegeman Avenue between Alabama and Malta. </t>
+  </si>
+  <si>
+    <t>I got pregnant in the ‘70s; I got pregnant at 17 in 1975 and my daughter born and then she passed away in Brookdale hospital. 
+Yes.  And that was painful.  And coming from a dysfunctional family, nobody knew how to hold each other up.  They knew how to cook for you, buy you clothes, I guess pay the rent, you know?  There wasn’t no hugging and kissing and all that stuff, that was abnormal in our house; that wasn’t a normal thing to do.  The normal thing to do was to feed you.  People have to eat, you know?  So it was just different.  And I got pregnant with my child in ’75 and I was heartbroken when she passed on, very, very heartbroken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We wanted to have a baby so then I found out that my tubes were blocked and I couldn't, so I went to, back then they had little clinics you could walk in off the street and they sent me to 59th Street and Columbus Circle to a big old building to do this procedure and they did this procedure where they shoot that dye inside you to see, and they told me that my tubes were blocked from the damage of the pregnancies…I had five pregnancies.  I had one child that passed and then through…. my behavior, I got pregnant so many times, so I damaged myself.  
+</t>
+  </si>
+  <si>
+    <t>I got up one morning, wasn’t thinking about (inaubible), I wasn’t thinking about it, I walked from 96th Street and Clarkson to Kings County Hospital.  And I sat in emergency and they called me, and I told them my history, and I want to have a baby and somebody told me there's a procedure that can be done.  They said yeah, we could do it.  And they gave me the appointment to come back and I went back and they did the procedure.  I got past the fifth month.  He said – if your water breaks, you're not meant to have a baby.  Got past the fifth month, got past the sixth month, got past the seventh month, but it didn't stop me.  I kept drugging.  I was gone.  I didn't have no attachment to the life that I was carrying.  I didn't have that attachment.  I was gone.  
+ I went in, my ninth month. August 6th and I had my queen.  They put the baby in my arms, she weighed 6 lbs. and 11 ounces, I didn't do no drugs for that week or so, so she didn't have no drugs in her system. Crack don’t stay long in your system. Had I not done drugs she probably would have been a real big baby because I love to eat anyway.  I didn't feel the love that a mother supposed to feel for this little thing.</t>
+  </si>
+  <si>
+    <t>So from there she went to Holliswood Hospital in Queens with all the different psych wards and stuff, and she’s suicidal, you know.  I knew then that I had to get myself together. I had to get myself together for my daughter.  Because she didn't deserve that, she didn’t deserve that, you know?  Having her on this earth for 12 years, some love for her, from me, kicked in, started kicking in.  Even though it wasn’t fully there and I didn't have that motherly instinct and stuff, but it was kicking in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coming out of this place they told me – did you hear about your daughter?  Because people been looking for you.  No, what happened to my daughter?  She’s in the hospital (crying) and in my brain I see my daughter hooked up to all these tubes and stuff.  I went home, the guy that let me sleep on the floor in his room, he let me in, because I went to the store for him that Monday and never came back with his money.  And he let me in and he told me – you need to get yourself together, go see your daughter.  She’s in King’s County, but she’s in the crazy house, the children’s crazy house. </t>
+  </si>
+  <si>
+    <t>I had her, I kept her around. I used to go to so many places and I used to take her with me.  She was like about eight months and I took her to a place and I guy sent me to get my drugs, to get us some drugs. I never went back (crying).  I never went back.  And somebody knew somebody who knew somebody who knew somebody who knew my husband, because I got married in ’90, and that’s when I found out I was HIV positive.  But he married me anyway.  I did the programs, I was clean and everything; in ’91 I went right back, I lost my daughter to the system.  Got my daughter back in’92 a year later, got her back but in the process of getting her back and going out to Amityville, Long Island to visit her in the foster care and the programs and stuff, I picked right back up, using.</t>
+  </si>
+  <si>
+    <t>I lived on the second floor.  I went to the bathroom and opened up the window, which fed the flames because there was smoke in my room.  The fire was behind the dresser but the windows and doors were closed, it was suffocating.  Fire cannot burn when it’s suffocating, it’s simmering right there.  When I opened up the windows and the air hit it, it just came up from behind the dresser and went towards the ceiling.
+I was laying there sleeping but I kept choking, I kept coughing because it was just smoke.  I left. I wasn’t going to go with the Red Cross.  The homicide, they investigated, they gave me a little interview and stuff.  I wasn’t going to go with the Red Cross, but I went with them, I went with the Red Cross anyway and they put me in a hotel.</t>
+  </si>
+  <si>
+    <t>And then I went into a program, because ACS got involved, and I went into a program.  I went to Kings County, the F Building or K Building whatever that is right there… entered program drug treatment
+And I went I there, and I sit there for three months and they're couldn't get me to say my name.  I wouldn't say my name because this is not where I want to be; I want to smoke drugs.  This is not the place I want to be.  But when I saw the people that came in there with me looked just as bad as I did, and three months went by, four months went by…five months, six months, seven months.  And- She gained some weight!  Her outfit is nice!  So I was putting on a little bit of weight and I started wanting what they had, you know?  I wanted to look nice. And I went straight from that little teeny woman to a size 20, I went straight up.  I felt good about myself.  But I still had low self-esteem.  Very low self-esteem.</t>
+  </si>
+  <si>
+    <t>My goal is, I know I'm ahead of time, but my goal is to bring awareness.  I live in Brownsville, Brooklyn.  My goal is to bring awareness to all the youth that’s out there.  Like I said before, I did meet Magic Johnson, he came to the church over there on Rochester and Dean Street.  He came over there and the questions that the young people had asked were so amazing because you look at a woman, the way that you are today, look at a woman and you can never tell what she have.</t>
+  </si>
+  <si>
+    <t>So my goal is, I want to speak, I want to bring something to my neighborhood and speak.  But if you know anything about Brownsville, there's a lot of killing going on, a lot of people with their turf, you live in that projects, I’m living over here, you're claiming your turf.  You wouldn't live there if your momma wasn’t paying the rent, you understand?  How can you claim government/city property?  That I can't walk through there.  So I'm afraid, I have a lot that I want to talk about in my community, anywhere, but I'm afraid.  My fear is that somebody’s going to hurt me if I come out with a certain message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have a lot of spiritual people that…Joyce McDonald from the Church of the Open Door, she does a lot of work…
+It’s on Gold Street, downtown.  I used to follow her everywhere she goes because her thing is from the shooting galleries to the art galleries.  If you see the art, the work that she’s done with her hands, the statues, you would think oh my gosh she bought it at a store…and she made it.  I used to go with her so many places when she going for her exhibits out there, I used to go with her.  She’s very, very beautiful.  And I want to be like that.  I used to follow her but life took me a different, different, different way.  I go up, I go down; I go up and I go down mentally, you know?
+</t>
+  </si>
+  <si>
+    <t>Oh, I have a beautiful support system, besides going to an NA or AA meeting, I have some sisters at Still I Rise, at Restoration that I spoke of earlier, we meet every Wednesday and we talk about so much stuff…our lives, our kids, our better halves.</t>
+  </si>
+  <si>
+    <t>HASA-- Also they pay your rent and they give you the funds, it’s different from welfare.  And it was hard for me to get HASA, because I am one of the non-progressives.  I have 20% of viral load or less, and it’s been this way since I became positive in ’89.  Never had an AIDS diagnosis.  So a lot of things was hard for me to get.  When I wanted to go into a program, programs back then was accepting everybody with AIDS.  But they will accept you if you have a mental disorder, and that’s how I got in the program, through the mental disorder.  That’s how I got HASA through my mental disorder, you understand me?  And then I was on a psychotropic medication, seroquil (sp?) I still take it today just to even me out.  I'm up sometimes, so many things it’s hard to get SSI, I couldn’t get it, they want you to-- and I'm glad.</t>
+  </si>
+  <si>
+    <t>When I started medication in ’99 it was crixivan and combivir.  Old medications; nobody’s using that today.  I just took myself off of crixivan, I told them I want to try something different, I don't know why.  They put me on Truvada, Norivan and Reyataz.  They’re the three that I’m on. So I have a lot of choices of different medications.  I just wanted to try something different.  The doctor put me on medication in ’99 when I got clean I went to the doctor…I said I’ve been positive now 10 years, could you give me something to boost my immune system.  He could have gave me some vitamin C, multi B vitamins, but he put me on these regimens.  I don't know why.  But I never took a holiday; I want to, but I never did.  I just started taking them.</t>
+  </si>
+  <si>
+    <t>Medical Treatment</t>
+  </si>
+  <si>
+    <t>That’s why in ’98 I had to have the hysterectomy because of so many surgeons…I had LEAP, I had laser, I had freezing.  And Downstate, they did the GYN twice a year.</t>
+  </si>
+  <si>
+    <t>there's a question in here asking about this Downstate, and I love Downstate because you know in ’87-’88 I think I must have contracted HPV, because I had very bad cervical dysplasia.</t>
+  </si>
+  <si>
+    <t>I had left Downstate for a moment and went over to Interfaith because it was next to the crack house.  When I went back to Interfaith in 2000, picked right back up with the doctor I had before, Barbara Sullivan, and she asked me why was I taking the medication?</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1094,24 +1099,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="43" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="J2" s="5">
         <v>1958</v>
@@ -1122,10 +1127,10 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E3" s="5">
         <v>40.680047600000002</v>
@@ -1140,18 +1145,18 @@
         <v>0</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="186.25" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E4" s="5">
         <v>40.659793000000001</v>
@@ -1163,13 +1168,13 @@
         <v>25</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -1177,27 +1182,27 @@
         <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="43" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E6" s="5">
         <v>40.658741999999997</v>
@@ -1209,7 +1214,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="43" x14ac:dyDescent="0.45">
@@ -1217,13 +1222,13 @@
         <v>62</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="E7" s="5">
         <v>40.747449500000002</v>
@@ -1238,18 +1243,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="257.85000000000002" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="E8" s="5">
         <v>40.662286100000003</v>
@@ -1264,35 +1269,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="171.9" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>70</v>
+        <v>194</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="5">
+        <v>40.654831100000003</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-73.912339099999997</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="143.25" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>95</v>
+        <v>195</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E10" s="5">
-        <v>40.654831100000003</v>
+        <v>40.7691996</v>
       </c>
       <c r="F10" s="5">
-        <v>-73.912339099999997</v>
+        <v>-73.984782800000005</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>26</v>
@@ -1301,24 +1321,24 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="286.5" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>128</v>
+        <v>196</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="E11" s="5">
-        <v>40.7691996</v>
+        <v>40.656601600000002</v>
       </c>
       <c r="F11" s="5">
-        <v>-73.984782800000005</v>
+        <v>-73.946227399999998</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>26</v>
@@ -1326,68 +1346,74 @@
       <c r="H11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J11" s="5">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="186.25" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="5">
-        <v>40.656601600000002</v>
-      </c>
-      <c r="F12" s="5">
-        <v>-73.946227399999998</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="143.25" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>104</v>
+        <v>198</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="5">
+        <v>40.656601600000002</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-73.946227399999998</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" ht="114.6" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>99</v>
+        <v>76</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="E14" s="5">
-        <v>40.656601600000002</v>
+        <v>40.718707700000003</v>
       </c>
       <c r="F14" s="5">
-        <v>-73.946227399999998</v>
+        <v>-73.770464099999998</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>26</v>
@@ -1395,48 +1421,39 @@
       <c r="H14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:12" ht="186.25" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="5">
-        <v>40.718707700000003</v>
-      </c>
-      <c r="F15" s="5">
-        <v>-73.770464099999998</v>
+        <v>200</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="243.55" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>201</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5">
+        <v>40.656601600000002</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-73.946227399999998</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>98</v>
+        <v>26</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
@@ -1444,91 +1461,88 @@
         <v>62</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="5">
-        <v>40.656601600000002</v>
-      </c>
-      <c r="F17" s="5">
-        <v>-73.946227399999998</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>26</v>
+        <v>65</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+      <c r="J17" s="5">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="114.6" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>106</v>
+        <v>93</v>
+      </c>
+      <c r="E18" s="5">
+        <v>40.6756593</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-73.927691300000006</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J18" s="5">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="200.55" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="E19" s="5">
-        <v>40.6756593</v>
+        <v>40.6986943</v>
       </c>
       <c r="F19" s="5">
-        <v>-73.927691300000006</v>
+        <v>-73.982801100000003</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="157.6" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="5">
-        <v>40.6986943</v>
-      </c>
-      <c r="F20" s="5">
-        <v>-73.982801100000003</v>
+        <v>77</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>113</v>
+        <v>69</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
@@ -1536,19 +1550,19 @@
         <v>62</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>25</v>
+        <v>66</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>107</v>
+        <v>85</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
@@ -1556,27 +1570,36 @@
         <v>62</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>102</v>
+        <v>67</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="57.3" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>84</v>
+        <v>205</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="5">
+        <v>40.6800353</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-73.945656999999997</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>37</v>
@@ -1585,147 +1608,154 @@
         <v>0</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="186.25" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E24" s="5">
-        <v>40.6800353</v>
-      </c>
-      <c r="F24" s="5">
-        <v>-73.945656999999997</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="171.9" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="J25" s="5">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+        <v>1999</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="71.650000000000006" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>108</v>
+        <v>211</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="5">
+        <v>40.678211300000001</v>
+      </c>
+      <c r="F26" s="5">
+        <v>-73.937531300000003</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="J26" s="5">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="43" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="5">
-        <v>40.678211300000001</v>
-      </c>
-      <c r="F27" s="5">
-        <v>-73.937531300000003</v>
-      </c>
-      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="1">
+        <v>40.6554</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-73.945700000000002</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A28" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="H27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="43" x14ac:dyDescent="0.45">
       <c r="B28" s="7" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="5">
-        <v>40.678211300000001</v>
-      </c>
-      <c r="F28" s="5">
-        <v>-73.937531300000003</v>
-      </c>
-      <c r="G28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="1">
+        <v>40.6554</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-73.945700000000002</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="71.650000000000006" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="D29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="1">
+        <v>40.6554</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-73.945700000000002</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>26</v>
+      <c r="H29" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2164,7 +2194,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2243,10 +2273,10 @@
     </row>
     <row r="3" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="E3" s="1">
         <v>40.670837800000001</v>
@@ -2261,18 +2291,18 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="E4" s="1">
         <v>40.651400700000003</v>
@@ -2289,13 +2319,13 @@
     </row>
     <row r="5" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E5" s="1">
         <v>40.671613200000003</v>
@@ -2312,13 +2342,13 @@
     </row>
     <row r="6" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="E6" s="1">
         <v>40.671613200000003</v>
@@ -2335,13 +2365,13 @@
     </row>
     <row r="7" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="E7" s="1">
         <v>40.673848800000002</v>
@@ -2358,13 +2388,13 @@
     </row>
     <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="E8" s="1">
         <v>40.681445199999999</v>
@@ -2381,10 +2411,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="J9" s="1">
         <v>1961</v>
@@ -2392,13 +2422,13 @@
     </row>
     <row r="10" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1">
         <v>40.655094200000001</v>
@@ -2421,13 +2451,13 @@
     </row>
     <row r="11" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="E11" s="1">
         <v>40.6924992</v>
@@ -2441,13 +2471,13 @@
     </row>
     <row r="12" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="E12" s="1">
         <v>40.674765999999998</v>
@@ -2456,7 +2486,7 @@
         <v>-73.874803499999999</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>0</v>
@@ -2464,7 +2494,7 @@
     </row>
     <row r="13" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>53</v>
@@ -2490,7 +2520,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>0</v>
@@ -2498,42 +2528,42 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="40" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="E19" s="1">
         <v>40.692163999999998</v>
@@ -2550,23 +2580,23 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2578,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2635,16 +2665,16 @@
     </row>
     <row r="2" spans="1:12" ht="66.349999999999994" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="E2" s="1">
         <v>40.860785800000002</v>
@@ -2659,18 +2689,18 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="J3" s="1">
         <v>1971</v>
@@ -2678,16 +2708,16 @@
     </row>
     <row r="4" spans="1:12" ht="53.15" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E4" s="1">
         <v>40.673837200000001</v>
@@ -2704,30 +2734,30 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="E6" s="1">
         <v>40.666868689130801</v>
@@ -2744,16 +2774,16 @@
     </row>
     <row r="7" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="E7" s="1">
         <v>40.657683909089997</v>
@@ -2770,16 +2800,16 @@
     </row>
     <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="E8" s="1">
         <v>40.640131529287601</v>
@@ -2796,10 +2826,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="J9" s="1">
         <v>1988</v>
@@ -2807,38 +2837,38 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="J11" s="1">
         <v>1994</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="J12" s="1">
         <v>1994</v>
@@ -2846,10 +2876,10 @@
     </row>
     <row r="13" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>37</v>
@@ -2863,13 +2893,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>0</v>
@@ -2877,30 +2907,30 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="26.8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E16" s="1">
         <v>40.792120500295397</v>
@@ -2909,38 +2939,38 @@
         <v>-73.886439153442296</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="40" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1">
         <v>40.655066400000003</v>
@@ -2960,24 +2990,24 @@
     </row>
     <row r="19" spans="1:11" ht="26.8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="J19" s="1">
         <v>1994</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>28</v>
@@ -2986,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>